<commit_message>
Visualize tax and other data on a map with python!
</commit_message>
<xml_diff>
--- a/popdata.xlsx
+++ b/popdata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Location</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Antigua, Alabama</t>
+  </si>
+  <si>
+    <t>https://plot.ly/~Dreamshot/9199/import-plotly-plotly-version-/#/</t>
   </si>
 </sst>
 </file>
@@ -490,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,6 +631,11 @@
         <v>-41.2</v>
       </c>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>